<commit_message>
BOM com capacitores mais baratos e com componentes que já temos na Control iD.
</commit_message>
<xml_diff>
--- a/Hardware/BOM-Proto-v3/BOM_LeitorRF_v3.xlsx
+++ b/Hardware/BOM-Proto-v3/BOM_LeitorRF_v3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="20190" windowHeight="8505" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="20190" windowHeight="8505" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="leitorcartao" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="LeitorRF_v3_FSK" sheetId="8" r:id="rId6"/>
     <sheet name="ListaTodosPN" sheetId="10" r:id="rId7"/>
     <sheet name="Consolidação" sheetId="13" r:id="rId8"/>
-    <sheet name="FinalDigikey" sheetId="14" r:id="rId9"/>
+    <sheet name="Pedido" sheetId="14" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">leitorcartao!$A$1:$V$167</definedName>
@@ -23,14 +23,14 @@
   </definedNames>
   <calcPr calcId="144525"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId10"/>
-    <pivotCache cacheId="11" r:id="rId11"/>
+    <pivotCache cacheId="0" r:id="rId10"/>
+    <pivotCache cacheId="1" r:id="rId11"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4361" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4361" uniqueCount="454">
   <si>
     <t>Part</t>
   </si>
@@ -1374,6 +1374,24 @@
   </si>
   <si>
     <t>DgkPN Proto</t>
+  </si>
+  <si>
+    <t>Retirar do pedido final</t>
+  </si>
+  <si>
+    <t>CL10C180FB8NNNC</t>
+  </si>
+  <si>
+    <t>1276-2206-1-ND</t>
+  </si>
+  <si>
+    <t>CL10C560FB8NNNC</t>
+  </si>
+  <si>
+    <t>1276-2312-1-ND</t>
+  </si>
+  <si>
+    <t>Obs.:</t>
   </si>
 </sst>
 </file>
@@ -4475,7 +4493,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:D60" firstHeaderRow="0" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
@@ -4857,7 +4875,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:D61" firstHeaderRow="0" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -5246,7 +5264,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:D63" firstHeaderRow="0" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -5934,8 +5952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V167"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N168" sqref="N168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -20324,7 +20342,7 @@
         <v>20</v>
       </c>
       <c r="G5" s="6">
-        <f t="shared" ref="G5:G61" si="0">$C$1*F5</f>
+        <f t="shared" ref="G5:G60" si="0">$C$1*F5</f>
         <v>120</v>
       </c>
       <c r="H5" s="6">
@@ -22614,8 +22632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B308"/>
   <sheetViews>
-    <sheetView topLeftCell="A190" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J150" sqref="J150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -25075,10 +25093,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J63"/>
+  <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K41" sqref="K41"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="K3" sqref="A3:K61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -25089,11 +25107,12 @@
     <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="9.33203125" style="6"/>
-    <col min="9" max="9" width="21.1640625" customWidth="1"/>
-    <col min="10" max="10" width="19.83203125" customWidth="1"/>
+    <col min="9" max="9" width="24.1640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C1" s="6" t="s">
         <v>413</v>
       </c>
@@ -25107,7 +25126,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>437</v>
       </c>
@@ -25132,14 +25151,17 @@
       <c r="H3" t="s">
         <v>445</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="9" t="s">
         <v>446</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="9" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3" s="9" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -25166,8 +25188,11 @@
         <f>IF(E4=1,MAX(G4+30,100),G4+5)</f>
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K4" s="9" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -25187,7 +25212,7 @@
         <v>37</v>
       </c>
       <c r="G5" s="6">
-        <f t="shared" ref="G5:G63" si="0">$D$1*F5</f>
+        <f t="shared" ref="G5:G61" si="0">$D$1*F5</f>
         <v>222</v>
       </c>
       <c r="H5">
@@ -25195,7 +25220,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>114</v>
       </c>
@@ -25223,7 +25248,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -25251,7 +25276,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -25278,11 +25303,11 @@
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="9" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>143</v>
       </c>
@@ -25309,11 +25334,11 @@
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="9" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -25340,11 +25365,14 @@
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
-      <c r="I10" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I10" s="9" t="s">
+        <v>449</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -25372,7 +25400,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>112</v>
       </c>
@@ -25399,11 +25427,11 @@
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="9" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>98</v>
       </c>
@@ -25431,7 +25459,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>83</v>
       </c>
@@ -25459,7 +25487,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>95</v>
       </c>
@@ -25487,7 +25515,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>70</v>
       </c>
@@ -25515,7 +25543,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>108</v>
       </c>
@@ -25543,7 +25571,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>74</v>
       </c>
@@ -25571,7 +25599,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -25599,7 +25627,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>121</v>
       </c>
@@ -25627,7 +25655,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>151</v>
       </c>
@@ -25654,11 +25682,14 @@
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="I21" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I21" s="9" t="s">
+        <v>451</v>
+      </c>
+      <c r="J21" s="9" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>104</v>
       </c>
@@ -25686,7 +25717,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>87</v>
       </c>
@@ -25714,7 +25745,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>181</v>
       </c>
@@ -25741,14 +25772,14 @@
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I24" s="9" t="s">
         <v>434</v>
       </c>
-      <c r="J24" t="s">
+      <c r="J24" s="9" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>167</v>
       </c>
@@ -25776,7 +25807,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>385</v>
       </c>
@@ -25804,7 +25835,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>390</v>
       </c>
@@ -25831,11 +25862,11 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I27" s="9" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>400</v>
       </c>
@@ -25862,8 +25893,11 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K28" s="9" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>395</v>
       </c>
@@ -25890,8 +25924,11 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K29" s="9" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>194</v>
       </c>
@@ -25919,7 +25956,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>209</v>
       </c>
@@ -25947,7 +25984,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>202</v>
       </c>
@@ -25974,7 +26011,7 @@
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="J32" t="s">
+      <c r="J32" s="9" t="s">
         <v>428</v>
       </c>
     </row>
@@ -26061,10 +26098,10 @@
         <f t="shared" si="1"/>
         <v>65</v>
       </c>
-      <c r="I35" t="s">
+      <c r="I35" s="9" t="s">
         <v>432</v>
       </c>
-      <c r="J35" t="s">
+      <c r="J35" s="9" t="s">
         <v>433</v>
       </c>
     </row>
@@ -26432,7 +26469,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>328</v>
       </c>
@@ -26460,7 +26497,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>303</v>
       </c>
@@ -26488,7 +26525,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>353</v>
       </c>
@@ -26516,7 +26553,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>265</v>
       </c>
@@ -26544,7 +26581,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>252</v>
       </c>
@@ -26572,7 +26609,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>312</v>
       </c>
@@ -26600,7 +26637,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>314</v>
       </c>
@@ -26628,7 +26665,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>319</v>
       </c>
@@ -26656,7 +26693,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>307</v>
       </c>
@@ -26684,7 +26721,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>282</v>
       </c>
@@ -26712,7 +26749,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>174</v>
       </c>
@@ -26740,7 +26777,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>247</v>
       </c>
@@ -26767,8 +26804,11 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K60" s="9" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>240</v>
       </c>
@@ -26796,7 +26836,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>439</v>
       </c>
@@ -26806,7 +26846,7 @@
       <c r="C62" s="8"/>
       <c r="D62" s="8"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>410</v>
       </c>
@@ -26819,22 +26859,22 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -26854,32 +26894,32 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="C2">
-        <v>17</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>114</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>115</v>
       </c>
       <c r="C3">
-        <v>252</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>114</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>115</v>
+        <v>42</v>
       </c>
       <c r="C4">
         <v>100</v>
@@ -26887,76 +26927,79 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s">
+        <v>422</v>
+      </c>
+      <c r="C5">
         <v>41</v>
-      </c>
-      <c r="B5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5">
-        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>143</v>
       </c>
       <c r="B6" t="s">
-        <v>422</v>
+        <v>430</v>
       </c>
       <c r="C6">
-        <v>41</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>143</v>
+        <v>62</v>
       </c>
       <c r="B7" t="s">
-        <v>430</v>
+        <v>449</v>
       </c>
       <c r="C7">
-        <v>29</v>
+        <v>77</v>
+      </c>
+      <c r="D7" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>424</v>
+        <v>35</v>
       </c>
       <c r="C8">
-        <v>77</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>112</v>
       </c>
       <c r="B9" t="s">
+        <v>426</v>
+      </c>
+      <c r="C9">
         <v>35</v>
-      </c>
-      <c r="C9">
-        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="B10" t="s">
-        <v>426</v>
+        <v>99</v>
       </c>
       <c r="C10">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="B11" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="C11">
         <v>17</v>
@@ -26964,10 +27007,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="B12" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="C12">
         <v>17</v>
@@ -26975,21 +27018,21 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="B13" t="s">
-        <v>96</v>
+        <v>71</v>
       </c>
       <c r="C13">
-        <v>17</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>70</v>
+        <v>108</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>109</v>
       </c>
       <c r="C14">
         <v>100</v>
@@ -26997,10 +27040,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>108</v>
+        <v>74</v>
       </c>
       <c r="B15" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
       <c r="C15">
         <v>100</v>
@@ -27008,54 +27051,57 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>74</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>75</v>
+        <v>32</v>
       </c>
       <c r="C16">
-        <v>100</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>121</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>122</v>
       </c>
       <c r="C17">
-        <v>29</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>121</v>
+        <v>151</v>
       </c>
       <c r="B18" t="s">
-        <v>122</v>
+        <v>451</v>
       </c>
       <c r="C18">
-        <v>100</v>
+        <v>29</v>
+      </c>
+      <c r="D18" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>151</v>
+        <v>104</v>
       </c>
       <c r="B19" t="s">
-        <v>425</v>
+        <v>105</v>
       </c>
       <c r="C19">
-        <v>29</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="B20" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="C20">
         <v>100</v>
@@ -27063,46 +27109,46 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>87</v>
+        <v>181</v>
       </c>
       <c r="B21" t="s">
-        <v>88</v>
+        <v>434</v>
       </c>
       <c r="C21">
-        <v>100</v>
+        <v>29</v>
+      </c>
+      <c r="D21" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="B22" t="s">
-        <v>434</v>
+        <v>168</v>
       </c>
       <c r="C22">
         <v>29</v>
       </c>
-      <c r="D22" t="s">
-        <v>435</v>
-      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>167</v>
+        <v>385</v>
       </c>
       <c r="B23" t="s">
-        <v>168</v>
+        <v>382</v>
       </c>
       <c r="C23">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>385</v>
+        <v>390</v>
       </c>
       <c r="B24" t="s">
-        <v>382</v>
+        <v>431</v>
       </c>
       <c r="C24">
         <v>17</v>
@@ -27110,82 +27156,82 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>390</v>
+        <v>194</v>
       </c>
       <c r="B25" t="s">
-        <v>387</v>
+        <v>195</v>
       </c>
       <c r="C25">
-        <v>17</v>
-      </c>
-      <c r="D25" t="s">
-        <v>431</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>400</v>
+        <v>209</v>
       </c>
       <c r="B26" t="s">
-        <v>401</v>
+        <v>210</v>
       </c>
       <c r="C26">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>395</v>
+        <v>202</v>
       </c>
       <c r="B27" t="s">
-        <v>392</v>
+        <v>203</v>
       </c>
       <c r="C27">
-        <v>17</v>
+        <v>29</v>
+      </c>
+      <c r="D27" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>194</v>
+        <v>216</v>
       </c>
       <c r="B28" t="s">
-        <v>195</v>
+        <v>215</v>
       </c>
       <c r="C28">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>209</v>
+        <v>221</v>
       </c>
       <c r="B29" t="s">
-        <v>210</v>
+        <v>222</v>
       </c>
       <c r="C29">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>202</v>
+        <v>225</v>
       </c>
       <c r="B30" t="s">
-        <v>203</v>
+        <v>432</v>
       </c>
       <c r="C30">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="D30" t="s">
-        <v>428</v>
+        <v>433</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>216</v>
+        <v>229</v>
       </c>
       <c r="B31" t="s">
-        <v>215</v>
+        <v>230</v>
       </c>
       <c r="C31">
         <v>17</v>
@@ -27193,200 +27239,197 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>221</v>
+        <v>273</v>
       </c>
       <c r="B32" t="s">
-        <v>222</v>
+        <v>274</v>
       </c>
       <c r="C32">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>225</v>
+        <v>277</v>
       </c>
       <c r="B33" t="s">
-        <v>432</v>
+        <v>278</v>
       </c>
       <c r="C33">
-        <v>65</v>
-      </c>
-      <c r="D33" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>229</v>
+        <v>341</v>
       </c>
       <c r="B34" t="s">
-        <v>230</v>
+        <v>342</v>
       </c>
       <c r="C34">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>273</v>
+        <v>298</v>
       </c>
       <c r="B35" t="s">
-        <v>274</v>
+        <v>299</v>
       </c>
       <c r="C35">
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>277</v>
+        <v>365</v>
       </c>
       <c r="B36" t="s">
-        <v>278</v>
+        <v>366</v>
       </c>
       <c r="C36">
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>341</v>
+        <v>257</v>
       </c>
       <c r="B37" t="s">
-        <v>342</v>
+        <v>258</v>
       </c>
       <c r="C37">
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>298</v>
+        <v>362</v>
       </c>
       <c r="B38" t="s">
-        <v>299</v>
+        <v>363</v>
       </c>
       <c r="C38">
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>365</v>
+        <v>286</v>
       </c>
       <c r="B39" t="s">
-        <v>366</v>
+        <v>287</v>
       </c>
       <c r="C39">
         <v>100</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>257</v>
+        <v>326</v>
       </c>
       <c r="B40" t="s">
-        <v>258</v>
+        <v>327</v>
       </c>
       <c r="C40">
         <v>100</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>362</v>
+        <v>261</v>
       </c>
       <c r="B41" t="s">
-        <v>363</v>
+        <v>262</v>
       </c>
       <c r="C41">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="B42" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
       <c r="C42">
         <v>100</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>326</v>
+        <v>269</v>
       </c>
       <c r="B43" t="s">
-        <v>327</v>
+        <v>270</v>
       </c>
       <c r="C43">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>328</v>
+      </c>
+      <c r="B44" t="s">
+        <v>329</v>
+      </c>
+      <c r="C44">
         <v>100</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>261</v>
-      </c>
-      <c r="B44" t="s">
-        <v>262</v>
-      </c>
-      <c r="C44">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>294</v>
+        <v>303</v>
       </c>
       <c r="B45" t="s">
-        <v>295</v>
+        <v>304</v>
       </c>
       <c r="C45">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>353</v>
+      </c>
+      <c r="B46" t="s">
+        <v>354</v>
+      </c>
+      <c r="C46">
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>269</v>
-      </c>
-      <c r="B46" t="s">
-        <v>270</v>
-      </c>
-      <c r="C46">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>328</v>
+        <v>265</v>
       </c>
       <c r="B47" t="s">
-        <v>329</v>
+        <v>266</v>
       </c>
       <c r="C47">
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>303</v>
+        <v>252</v>
       </c>
       <c r="B48" t="s">
-        <v>304</v>
+        <v>253</v>
       </c>
       <c r="C48">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>353</v>
+        <v>312</v>
       </c>
       <c r="B49" t="s">
-        <v>354</v>
+        <v>313</v>
       </c>
       <c r="C49">
         <v>100</v>
@@ -27394,10 +27437,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>265</v>
+        <v>314</v>
       </c>
       <c r="B50" t="s">
-        <v>266</v>
+        <v>315</v>
       </c>
       <c r="C50">
         <v>100</v>
@@ -27405,10 +27448,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>252</v>
+        <v>319</v>
       </c>
       <c r="B51" t="s">
-        <v>253</v>
+        <v>320</v>
       </c>
       <c r="C51">
         <v>100</v>
@@ -27416,10 +27459,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="B52" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="C52">
         <v>100</v>
@@ -27427,10 +27470,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>314</v>
+        <v>282</v>
       </c>
       <c r="B53" t="s">
-        <v>315</v>
+        <v>283</v>
       </c>
       <c r="C53">
         <v>100</v>
@@ -27438,67 +27481,23 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>319</v>
+        <v>174</v>
       </c>
       <c r="B54" t="s">
-        <v>320</v>
+        <v>175</v>
       </c>
       <c r="C54">
-        <v>100</v>
+        <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>307</v>
+        <v>240</v>
       </c>
       <c r="B55" t="s">
-        <v>308</v>
+        <v>241</v>
       </c>
       <c r="C55">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>282</v>
-      </c>
-      <c r="B56" t="s">
-        <v>283</v>
-      </c>
-      <c r="C56">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>174</v>
-      </c>
-      <c r="B57" t="s">
-        <v>175</v>
-      </c>
-      <c r="C57">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>247</v>
-      </c>
-      <c r="B58" t="s">
-        <v>248</v>
-      </c>
-      <c r="C58">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>240</v>
-      </c>
-      <c r="B59" t="s">
-        <v>241</v>
-      </c>
-      <c r="C59">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Troca do capacitor do circuito tanque que estava fora de estoque.
</commit_message>
<xml_diff>
--- a/Hardware/BOM-Proto-v3/BOM_LeitorRF_v3.xlsx
+++ b/Hardware/BOM-Proto-v3/BOM_LeitorRF_v3.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4361" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4364" uniqueCount="456">
   <si>
     <t>Part</t>
   </si>
@@ -1392,6 +1392,12 @@
   </si>
   <si>
     <t>Obs.:</t>
+  </si>
+  <si>
+    <t>C1210C102FBGACTU</t>
+  </si>
+  <si>
+    <t>399-5548-1-ND</t>
   </si>
 </sst>
 </file>
@@ -25095,8 +25101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="K3" sqref="A3:K61"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -25486,6 +25492,12 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
+      <c r="I14" s="9" t="s">
+        <v>454</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>455</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -26868,7 +26880,7 @@
   <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -26998,11 +27010,14 @@
       <c r="A11" t="s">
         <v>83</v>
       </c>
-      <c r="B11" t="s">
-        <v>84</v>
+      <c r="B11" s="9" t="s">
+        <v>454</v>
       </c>
       <c r="C11">
         <v>17</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>